<commit_message>
successfully added an image for a practitioner. need to add the rest of the images next
</commit_message>
<xml_diff>
--- a/public/data/practitioners.xlsx
+++ b/public/data/practitioners.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianlalli/Desktop/NewCo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C516B60A-EA78-9D43-9A03-EE7A541584F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{317A1A33-CB86-FF4C-8F87-EAD4BB2CBBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="1210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2977" uniqueCount="1212">
   <si>
     <t>Clinic/s</t>
   </si>
@@ -3707,6 +3707,12 @@
   </si>
   <si>
     <t>Acupuncturist</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>https://www.carechiropractic.com/wp-content/uploads/2018/02/about_drv3.jpg.webp</t>
   </si>
 </sst>
 </file>
@@ -4847,8 +4853,8 @@
   </sheetPr>
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C23"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4857,6 +4863,7 @@
     <col min="5" max="5" width="11.1640625" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="19" max="19" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1">
@@ -4914,6 +4921,9 @@
       <c r="R1" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="S1" s="4" t="s">
+        <v>1210</v>
+      </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -4966,7 +4976,9 @@
       <c r="R2" s="7">
         <v>80220</v>
       </c>
-      <c r="S2" s="7"/>
+      <c r="S2" s="7" t="s">
+        <v>1211</v>
+      </c>
       <c r="T2" s="11"/>
       <c r="U2" s="7"/>
     </row>

</xml_diff>

<commit_message>
started development of matching algo. updated social links as well
</commit_message>
<xml_diff>
--- a/public/data/practitioners.xlsx
+++ b/public/data/practitioners.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianlalli/Desktop/NewCo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8895299-A4BB-074A-976F-91DB594ED0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{937D7954-707A-8D4A-8481-7D8F49BB6F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2998" uniqueCount="1232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="1233">
   <si>
     <t>Clinic/s</t>
   </si>
@@ -3773,6 +3773,9 @@
   </si>
   <si>
     <t>https://photos.healthprofs.com/583d838d-46cd-11ea-a6ad-06142c356176/3/320x400.jpeg</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -4912,1389 +4915,1459 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="19" max="19" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="20" max="20" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" customHeight="1">
+    <row r="1" spans="1:22" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1205</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>1209</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A2" s="168">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="168" t="s">
+      <c r="C2" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>1206</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="7">
+      <c r="F2" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F2" s="7">
+      <c r="G2" s="7">
         <v>408</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="10"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="7" t="s">
+      <c r="M2" s="10"/>
+      <c r="N2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="7">
+      <c r="R2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="7">
         <v>80220</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>1228</v>
       </c>
-      <c r="T2" s="11"/>
-      <c r="U2" s="7"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="U2" s="11"/>
+      <c r="V2" s="7"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A3" s="168">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="168" t="s">
+      <c r="C3" s="168" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>1206</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="7">
+      <c r="F3" s="7">
         <v>4.8</v>
       </c>
-      <c r="F3" s="7">
+      <c r="G3" s="7">
         <v>401</v>
       </c>
-      <c r="G3" s="7">
+      <c r="H3" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="H3" s="7">
+      <c r="I3" s="7">
         <v>39</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="N3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" s="7">
+      <c r="R3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="7">
         <v>80401</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="T3" s="7" t="s">
         <v>1210</v>
       </c>
-      <c r="T3" s="11"/>
-      <c r="U3" s="13"/>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="U3" s="11"/>
+      <c r="V3" s="13"/>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A4" s="168">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="168" t="s">
+      <c r="C4" s="168" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>1206</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="7">
+      <c r="F4" s="7">
         <v>4.8</v>
       </c>
-      <c r="F4" s="7">
+      <c r="G4" s="7">
         <v>401</v>
       </c>
-      <c r="G4" s="7">
+      <c r="H4" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H4" s="7">
+      <c r="I4" s="7">
         <v>12</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="L4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="M4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="N4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="Q4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="7">
+      <c r="R4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="7">
         <v>80401</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="T4" s="7" t="s">
         <v>1211</v>
       </c>
-      <c r="T4" s="11"/>
-      <c r="U4" s="13"/>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="U4" s="11"/>
+      <c r="V4" s="13"/>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A5" s="168">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="168" t="s">
+      <c r="C5" s="168" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>1206</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="7">
         <v>4.8</v>
       </c>
-      <c r="F5" s="7">
+      <c r="G5" s="7">
         <v>401</v>
       </c>
-      <c r="G5" s="7">
+      <c r="H5" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H5" s="7">
+      <c r="I5" s="7">
         <v>35</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="L5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="M5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="N5" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="P5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R5" s="7">
+      <c r="R5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="7">
         <v>80401</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="T5" s="7" t="s">
         <v>1229</v>
       </c>
-      <c r="T5" s="11"/>
-      <c r="U5" s="13"/>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="U5" s="11"/>
+      <c r="V5" s="13"/>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A6" s="168">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="168" t="s">
+      <c r="C6" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>1206</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="7">
+      <c r="F6" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F6" s="7">
+      <c r="G6" s="7">
         <v>374</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="K6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="L6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="10"/>
+      <c r="N6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="P6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="Q6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Q6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R6" s="7">
+      <c r="R6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" s="7">
         <v>80246</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="T6" s="7" t="s">
         <v>1212</v>
       </c>
-      <c r="T6" s="11"/>
-      <c r="U6" s="13"/>
-    </row>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="U6" s="11"/>
+      <c r="V6" s="13"/>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A7" s="168">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="168" t="s">
+      <c r="C7" s="168" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>1206</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="7">
+      <c r="F7" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="7">
         <v>374</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="L7" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="10"/>
+      <c r="N7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="O7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="P7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="Q7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Q7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R7" s="7">
+      <c r="R7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="7">
         <v>80246</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="T7" s="7" t="s">
         <v>1213</v>
       </c>
-      <c r="T7" s="11"/>
-      <c r="U7" s="13"/>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="U7" s="11"/>
+      <c r="V7" s="13"/>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A8" s="168">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="168" t="s">
+      <c r="C8" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>1206</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="7">
+      <c r="F8" s="7">
         <v>5</v>
       </c>
-      <c r="F8" s="7">
+      <c r="G8" s="7">
         <v>353</v>
       </c>
-      <c r="G8" s="7">
+      <c r="H8" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H8" s="7">
+      <c r="I8" s="7">
         <v>12</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="K8" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="L8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="12" t="s">
+      <c r="M8" s="10"/>
+      <c r="N8" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="O8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="P8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="Q8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="Q8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R8" s="7">
+      <c r="R8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" s="7">
         <v>80111</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="T8" s="7" t="s">
         <v>1214</v>
       </c>
-      <c r="T8" s="11"/>
-      <c r="U8" s="13"/>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="U8" s="11"/>
+      <c r="V8" s="13"/>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A9" s="168">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="168" t="s">
+      <c r="C9" s="168" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>1206</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="7">
+      <c r="F9" s="7">
         <v>5</v>
       </c>
-      <c r="F9" s="7">
+      <c r="G9" s="7">
         <v>353</v>
       </c>
-      <c r="G9" s="7">
+      <c r="H9" s="7">
         <v>4.8</v>
       </c>
-      <c r="H9" s="7">
+      <c r="I9" s="7">
         <v>12</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="K9" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="L9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="12" t="s">
+      <c r="M9" s="10"/>
+      <c r="N9" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="N9" s="7" t="s">
+      <c r="O9" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="O9" s="7" t="s">
+      <c r="P9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="Q9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="Q9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9" s="7">
+      <c r="R9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" s="7">
         <v>80111</v>
       </c>
-      <c r="S9" s="7" t="s">
+      <c r="T9" s="7" t="s">
         <v>1215</v>
       </c>
-      <c r="T9" s="11"/>
-      <c r="U9" s="7"/>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="U9" s="11"/>
+      <c r="V9" s="7"/>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A10" s="168">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="168" t="s">
+      <c r="C10" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>1207</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="7">
+      <c r="F10" s="7">
         <v>4.8</v>
       </c>
-      <c r="F10" s="7">
+      <c r="G10" s="7">
         <v>165</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="K10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="L10" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="10"/>
+      <c r="N10" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="O10" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O10" s="7" t="s">
+      <c r="P10" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="P10" s="7" t="s">
+      <c r="Q10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Q10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R10" s="7">
+      <c r="R10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="7">
         <v>80246</v>
       </c>
-      <c r="S10" s="7" t="s">
+      <c r="T10" s="7" t="s">
         <v>1216</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A11" s="168">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="168" t="s">
+      <c r="C11" s="168" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>1207</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="7">
+      <c r="F11" s="7">
         <v>5</v>
       </c>
-      <c r="F11" s="14">
+      <c r="G11" s="14">
         <v>153</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="K11" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="L11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="M11" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="12" t="s">
+      <c r="N11" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="N11" s="7" t="s">
+      <c r="O11" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="P11" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="P11" s="7" t="s">
+      <c r="Q11" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="Q11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R11" s="7">
+      <c r="R11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S11" s="7">
         <v>80214</v>
       </c>
-      <c r="S11" s="7" t="s">
+      <c r="T11" s="7" t="s">
         <v>1217</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A12" s="168">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="168" t="s">
+      <c r="C12" s="168" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>1207</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="7">
+      <c r="F12" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F12" s="7">
+      <c r="G12" s="7">
         <v>72</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="K12" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="L12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="M12" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="N12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="N12" s="7" t="s">
+      <c r="O12" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="O12" s="7" t="s">
+      <c r="P12" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="P12" s="7" t="s">
+      <c r="Q12" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R12" s="7">
+      <c r="R12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S12" s="7">
         <v>80003</v>
       </c>
-      <c r="S12" s="7" t="s">
+      <c r="T12" s="7" t="s">
         <v>1218</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A13" s="168">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="168" t="s">
+      <c r="C13" s="168" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>1207</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="7">
+      <c r="F13" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F13" s="7">
+      <c r="G13" s="7">
         <v>59</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="K13" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="L13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="10"/>
-      <c r="M13" s="12" t="s">
+      <c r="M13" s="10"/>
+      <c r="N13" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="N13" s="7" t="s">
+      <c r="O13" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="O13" s="7" t="s">
+      <c r="P13" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="P13" s="7" t="s">
+      <c r="Q13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Q13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R13" s="7">
+      <c r="R13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13" s="7">
         <v>80209</v>
       </c>
-      <c r="S13" s="7" t="s">
+      <c r="T13" s="7" t="s">
         <v>1231</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A14" s="168">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="168" t="s">
+      <c r="C14" s="168" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>1207</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="7">
+      <c r="F14" s="7">
         <v>5</v>
       </c>
-      <c r="F14" s="7">
+      <c r="G14" s="7">
         <v>27</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="K14" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="L14" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="M14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="12" t="s">
+      <c r="N14" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="N14" s="7" t="s">
+      <c r="O14" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="O14" s="7" t="s">
+      <c r="P14" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="P14" s="7" t="s">
+      <c r="Q14" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="Q14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R14" s="7">
+      <c r="R14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S14" s="7">
         <v>80215</v>
       </c>
-      <c r="S14" s="7" t="s">
+      <c r="T14" s="7" t="s">
         <v>1219</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A15" s="168">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="168" t="s">
+      <c r="C15" s="168" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>1207</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="7">
+      <c r="F15" s="7">
         <v>5</v>
       </c>
-      <c r="F15" s="7">
-        <v>26</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>20</v>
+      <c r="G15" s="7">
+        <v>26</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="K15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="10" t="s">
+      <c r="L15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="12" t="s">
+      <c r="N15" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="N15" s="7" t="s">
+      <c r="O15" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="O15" s="7" t="s">
+      <c r="P15" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="P15" s="7" t="s">
+      <c r="Q15" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="Q15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R15" s="7">
+      <c r="R15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S15" s="7">
         <v>80033</v>
       </c>
-      <c r="S15" s="7" t="s">
+      <c r="T15" s="7" t="s">
         <v>1230</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A16" s="168">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="168" t="s">
+      <c r="C16" s="168" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>1207</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="7">
+      <c r="F16" s="7">
         <v>5</v>
       </c>
-      <c r="F16" s="7">
+      <c r="G16" s="7">
         <v>13</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="K16" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="L16" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="M16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="12" t="s">
+      <c r="N16" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="N16" s="7" t="s">
+      <c r="O16" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="O16" s="7" t="s">
+      <c r="P16" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="P16" s="7" t="s">
+      <c r="Q16" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="Q16" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R16" s="7">
+      <c r="R16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S16" s="7">
         <v>80033</v>
       </c>
-      <c r="S16" s="7" t="s">
+      <c r="T16" s="7" t="s">
         <v>1220</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A17" s="168">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="168" t="s">
+      <c r="C17" s="168" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>1207</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="7">
+      <c r="F17" s="7">
         <v>5</v>
       </c>
-      <c r="F17" s="7">
+      <c r="G17" s="7">
         <v>21</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="K17" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>119</v>
       </c>
       <c r="L17" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="M17" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="N17" s="7" t="s">
+      <c r="M17" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="O17" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="O17" s="7" t="s">
+      <c r="P17" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="7" t="s">
+      <c r="Q17" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R17" s="7">
+      <c r="R17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S17" s="7">
         <v>80214</v>
       </c>
-      <c r="S17" s="7" t="s">
+      <c r="T17" s="7" t="s">
         <v>1221</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A18" s="168">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B18" s="168" t="s">
+      <c r="C18" s="168" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>1208</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="E18" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="E18" s="7">
+      <c r="F18" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F18" s="7">
+      <c r="G18" s="7">
         <v>866</v>
       </c>
-      <c r="G18" s="13"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="16" t="s">
+      <c r="I18" s="13"/>
+      <c r="J18" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="K18" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="N18" s="13"/>
+      <c r="N18" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
       <c r="R18" s="13"/>
-      <c r="S18" s="7" t="s">
+      <c r="S18" s="13"/>
+      <c r="T18" s="7" t="s">
         <v>1222</v>
       </c>
-      <c r="T18" s="13"/>
-    </row>
-    <row r="19" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A19" s="6" t="s">
+      <c r="U18" s="13"/>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A19" s="168">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="168" t="s">
+      <c r="C19" s="168" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>1208</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="7">
+      <c r="F19" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F19" s="7">
+      <c r="G19" s="7">
         <v>331</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="K19" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M19" s="12" t="s">
+      <c r="N19" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="N19" s="7" t="s">
+      <c r="O19" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="O19" s="7" t="s">
+      <c r="P19" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="P19" s="7" t="s">
+      <c r="Q19" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="Q19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R19" s="7">
+      <c r="R19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S19" s="7">
         <v>80004</v>
       </c>
-      <c r="S19" s="7" t="s">
+      <c r="T19" s="7" t="s">
         <v>1223</v>
       </c>
-      <c r="T19" s="13"/>
-    </row>
-    <row r="20" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A20" s="6" t="s">
+      <c r="U19" s="13"/>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A20" s="168">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B20" s="168" t="s">
+      <c r="C20" s="168" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>1208</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E20" s="7">
+      <c r="F20" s="7">
         <v>5</v>
       </c>
-      <c r="F20" s="7">
+      <c r="G20" s="7">
         <v>262</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="K20" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="L20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="M20" s="12" t="s">
+      <c r="N20" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="N20" s="7" t="s">
+      <c r="O20" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="O20" s="7" t="s">
+      <c r="P20" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="P20" s="7" t="s">
+      <c r="Q20" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="Q20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R20" s="7">
+      <c r="R20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S20" s="7">
         <v>80138</v>
       </c>
-      <c r="S20" s="7" t="s">
+      <c r="T20" s="7" t="s">
         <v>1224</v>
       </c>
-      <c r="T20" s="13"/>
-    </row>
-    <row r="21" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A21" s="6" t="s">
+      <c r="U20" s="13"/>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A21" s="168">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B21" s="168" t="s">
+      <c r="C21" s="168" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>1208</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E21" s="7">
+      <c r="F21" s="7">
         <v>5</v>
       </c>
-      <c r="F21" s="7">
+      <c r="G21" s="7">
         <v>262</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H21" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="K21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="10" t="s">
+      <c r="L21" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="M21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="N21" s="7" t="s">
+      <c r="N21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="O21" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="O21" s="7" t="s">
+      <c r="P21" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="P21" s="7" t="s">
+      <c r="Q21" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="Q21" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R21" s="7">
+      <c r="R21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S21" s="7">
         <v>80138</v>
       </c>
-      <c r="S21" s="7" t="s">
+      <c r="T21" s="7" t="s">
         <v>1227</v>
       </c>
-      <c r="T21" s="13"/>
-    </row>
-    <row r="22" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A22" s="6" t="s">
+      <c r="U21" s="13"/>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A22" s="168">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B22" s="168" t="s">
+      <c r="C22" s="168" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>1208</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="7">
+      <c r="F22" s="7">
         <v>4.8</v>
       </c>
-      <c r="F22" s="7">
+      <c r="G22" s="7">
         <v>178</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="K22" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K22" s="10" t="s">
+      <c r="L22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="M22" s="12" t="s">
+      <c r="N22" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="N22" s="7" t="s">
+      <c r="O22" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="O22" s="7" t="s">
+      <c r="P22" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="P22" s="7" t="s">
+      <c r="Q22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Q22" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R22" s="7">
+      <c r="R22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S22" s="7">
         <v>80203</v>
       </c>
-      <c r="S22" s="7" t="s">
+      <c r="T22" s="7" t="s">
         <v>1225</v>
       </c>
-      <c r="T22" s="13"/>
-    </row>
-    <row r="23" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="U22" s="13"/>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A23" s="168">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B23" s="168" t="s">
+      <c r="C23" s="168" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>1208</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="7">
+      <c r="F23" s="7">
         <v>4.8</v>
       </c>
-      <c r="F23" s="7">
+      <c r="G23" s="7">
         <v>178</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="H23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="J23" s="10" t="s">
+      <c r="K23" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="L23" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="M23" s="12" t="s">
+      <c r="N23" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="N23" s="7" t="s">
+      <c r="O23" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="O23" s="7" t="s">
+      <c r="P23" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="P23" s="7" t="s">
+      <c r="Q23" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Q23" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R23" s="7">
+      <c r="R23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S23" s="7">
         <v>80203</v>
       </c>
-      <c r="S23" s="7" t="s">
+      <c r="T23" s="7" t="s">
         <v>1226</v>
       </c>
-      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="D4" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="I4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="D5" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="I5" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="D6" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="I6" r:id="rId10" location="chiro-apt" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="I7" r:id="rId12" location="chiro-apt" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="D8" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="I8" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="D9" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="I9" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="I18" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="D19" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="I19" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="D20" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="I20" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="D21" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="I21" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="D22" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="I22" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="D23" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="I23" r:id="rId28" location="/staff_member/3" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="I17" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="D17" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="I16" r:id="rId31" location="/team" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="D16" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="I15" r:id="rId33" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="D15" r:id="rId34" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="I14" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="D14" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="I13" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="D13" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="I12" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="D12" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="I11" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="D11" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="I10" r:id="rId43" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="D10" r:id="rId44" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="J3" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="J4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="J5" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E6" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="J6" r:id="rId10" location="chiro-apt" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E7" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="J7" r:id="rId12" location="chiro-apt" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="E8" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="J8" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="E9" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="J9" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="J18" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="E19" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="J19" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="E20" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="J20" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="E21" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="J21" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="E22" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="J22" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="E23" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="J23" r:id="rId28" location="/staff_member/3" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="J17" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="E17" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="J16" r:id="rId31" location="/team" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="E16" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="J15" r:id="rId33" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="E15" r:id="rId34" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="J14" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="E14" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="J13" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="E13" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="J12" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="E12" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="J11" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="E11" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="J10" r:id="rId43" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="E10" r:id="rId44" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added another zip code and it looks like all practitioners locations are being calculated. also tweaked the quiz questions logic to remove branching after Q1. lastly I tweaked answers to questions 3 and 4 to better align with logic.
</commit_message>
<xml_diff>
--- a/public/data/practitioners.xlsx
+++ b/public/data/practitioners.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianlalli/Desktop/NewCo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE9C0F5F-7EA3-4141-BB6B-3472A3F3B0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8EEAE5D-98CC-1E40-B39B-79415608DC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="1640" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MVP Practitioners" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Massage Therapists'!$A$3:$R$125</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Prospects List'!$A$7:$AE$160</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Zip Code Infrastructure'!$A$1:$E$999</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Zip Code Infrastructure'!$A$1:$E$1000</definedName>
     <definedName name="Z_2D114C46_41D7_4FBC_B93A_EDECFD188CDF_.wvu.FilterData" localSheetId="5" hidden="1">'Prospects List'!$A$7:$AE$160</definedName>
     <definedName name="Z_4DADA64F_E99D_4560_8154_F4711FEFCC09_.wvu.FilterData" localSheetId="5" hidden="1">'Prospects List'!$A$1:$AE$160</definedName>
     <definedName name="Z_54CD2F5B_55D9_4191_B81C_1C02D9A49EAE_.wvu.FilterData" localSheetId="5" hidden="1">'Prospects List'!$A$1:$AE$160</definedName>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3007" uniqueCount="1236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3012" uniqueCount="1238">
   <si>
     <t>Clinic/s</t>
   </si>
@@ -3785,6 +3785,12 @@
   </si>
   <si>
     <t>drtrent@denverchiropracticllc.com</t>
+  </si>
+  <si>
+    <t>Elevation Chiropractic and Wellness</t>
+  </si>
+  <si>
+    <t>Pain</t>
   </si>
 </sst>
 </file>
@@ -4926,14 +4932,14 @@
   </sheetPr>
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" customWidth="1"/>
     <col min="7" max="7" width="9.1640625" customWidth="1"/>
     <col min="8" max="8" width="11.5" customWidth="1"/>
@@ -5037,7 +5043,9 @@
       <c r="K2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="10"/>
+      <c r="L2" s="10" t="s">
+        <v>1237</v>
+      </c>
       <c r="M2" s="10"/>
       <c r="N2" s="9" t="s">
         <v>20</v>
@@ -5260,7 +5268,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>41</v>
+        <v>1236</v>
       </c>
       <c r="C6" s="168" t="s">
         <v>42</v>
@@ -5322,7 +5330,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>41</v>
+        <v>1236</v>
       </c>
       <c r="C7" s="168" t="s">
         <v>49</v>
@@ -6026,6 +6034,9 @@
       <c r="K18" s="10" t="s">
         <v>22</v>
       </c>
+      <c r="L18" s="10" t="s">
+        <v>1237</v>
+      </c>
       <c r="N18" s="12" t="s">
         <v>1235</v>
       </c>
@@ -6082,6 +6093,9 @@
       </c>
       <c r="K19" s="10" t="s">
         <v>22</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>1237</v>
       </c>
       <c r="N19" s="12" t="s">
         <v>129</v>
@@ -6402,10 +6416,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L341"/>
+  <dimension ref="A1:R341"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -8462,7 +8476,7 @@
         <v>-104.77</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15">
+    <row r="65" spans="1:18" ht="15">
       <c r="A65" s="18">
         <v>80125</v>
       </c>
@@ -8494,7 +8508,7 @@
         <v>-104.72199999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15">
+    <row r="66" spans="1:18" ht="15">
       <c r="A66" s="18">
         <v>80127</v>
       </c>
@@ -8526,7 +8540,7 @@
         <v>-104.71299999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15">
+    <row r="67" spans="1:18" ht="15">
       <c r="A67" s="18">
         <v>80501</v>
       </c>
@@ -8558,7 +8572,7 @@
         <v>-104.74</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15">
+    <row r="68" spans="1:18" ht="15">
       <c r="A68" s="18">
         <v>80503</v>
       </c>
@@ -8589,8 +8603,11 @@
       <c r="L68" s="20">
         <v>-104.74</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" ht="15">
+      <c r="P68" s="7"/>
+      <c r="Q68" s="7"/>
+      <c r="R68" s="7"/>
+    </row>
+    <row r="69" spans="1:18" ht="15">
       <c r="A69" s="18">
         <v>80504</v>
       </c>
@@ -8622,7 +8639,7 @@
         <v>-104.773</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15">
+    <row r="70" spans="1:18" ht="15">
       <c r="A70" s="18">
         <v>80465</v>
       </c>
@@ -8654,7 +8671,7 @@
         <v>-104.846</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15">
+    <row r="71" spans="1:18" ht="15">
       <c r="A71" s="18">
         <v>80233</v>
       </c>
@@ -8686,7 +8703,7 @@
         <v>-104.767</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15">
+    <row r="72" spans="1:18" ht="15">
       <c r="A72" s="18">
         <v>80234</v>
       </c>
@@ -8718,7 +8735,7 @@
         <v>-104.81399999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15">
+    <row r="73" spans="1:18" ht="15">
       <c r="A73" s="18">
         <v>80241</v>
       </c>
@@ -8750,7 +8767,7 @@
         <v>-104.69799999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15">
+    <row r="74" spans="1:18" ht="15">
       <c r="A74" s="18">
         <v>80134</v>
       </c>
@@ -8782,21 +8799,21 @@
         <v>-104.66</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15">
+    <row r="75" spans="1:18" ht="15">
       <c r="A75" s="18">
-        <v>80229</v>
+        <v>80138</v>
       </c>
       <c r="B75" s="19" t="s">
         <v>26</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>229</v>
+        <v>139</v>
       </c>
       <c r="D75" s="18">
-        <v>39.860999999999997</v>
+        <v>39.511600000000001</v>
       </c>
       <c r="E75" s="18">
-        <v>-104.962</v>
+        <v>-104.69029999999999</v>
       </c>
       <c r="H75" s="20">
         <v>80926</v>
@@ -8814,21 +8831,21 @@
         <v>-104.851</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15">
+    <row r="76" spans="1:18" ht="15">
       <c r="A76" s="18">
-        <v>80021</v>
+        <v>80229</v>
       </c>
       <c r="B76" s="19" t="s">
         <v>26</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D76" s="18">
-        <v>39.875999999999998</v>
+        <v>39.860999999999997</v>
       </c>
       <c r="E76" s="18">
-        <v>-105.10299999999999</v>
+        <v>-104.962</v>
       </c>
       <c r="H76" s="20">
         <v>80928</v>
@@ -8846,9 +8863,9 @@
         <v>-104.45699999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15">
+    <row r="77" spans="1:18" ht="15">
       <c r="A77" s="18">
-        <v>80030</v>
+        <v>80021</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>26</v>
@@ -8857,10 +8874,10 @@
         <v>230</v>
       </c>
       <c r="D77" s="18">
-        <v>39.854239999999997</v>
+        <v>39.875999999999998</v>
       </c>
       <c r="E77" s="18">
-        <v>-105.03700000000001</v>
+        <v>-105.10299999999999</v>
       </c>
       <c r="H77" s="20">
         <v>80929</v>
@@ -8878,21 +8895,21 @@
         <v>-104.608</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15">
+    <row r="78" spans="1:18" ht="15">
       <c r="A78" s="18">
-        <v>80033</v>
+        <v>80030</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>26</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>106</v>
+        <v>230</v>
       </c>
       <c r="D78" s="18">
-        <v>39.774039999999999</v>
+        <v>39.854239999999997</v>
       </c>
       <c r="E78" s="18">
-        <v>-105.096</v>
+        <v>-105.03700000000001</v>
       </c>
       <c r="H78" s="20">
         <v>80930</v>
@@ -8910,7 +8927,22 @@
         <v>-104.527</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15">
+    <row r="79" spans="1:18" ht="15">
+      <c r="A79" s="18">
+        <v>80033</v>
+      </c>
+      <c r="B79" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D79" s="18">
+        <v>39.774039999999999</v>
+      </c>
+      <c r="E79" s="18">
+        <v>-105.096</v>
+      </c>
       <c r="H79" s="20">
         <v>80022</v>
       </c>
@@ -8927,7 +8959,7 @@
         <v>-104.911</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15">
+    <row r="80" spans="1:18" ht="15">
       <c r="H80" s="20">
         <v>80433</v>
       </c>
@@ -13350,7 +13382,7 @@
     <row r="340" spans="8:12" ht="13"/>
     <row r="341" spans="8:12" ht="13"/>
   </sheetData>
-  <autoFilter ref="A1:E999" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:E1000" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated styling on practitioners page
</commit_message>
<xml_diff>
--- a/public/data/practitioners.xlsx
+++ b/public/data/practitioners.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianlalli/Desktop/NewCo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianlalli/Desktop/Natu.Health/Natu.Health/public/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8EEAE5D-98CC-1E40-B39B-79415608DC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F5A9CB-9E38-9042-BC3F-AD1770D76099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="1640" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,16 +38,15 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 6" guid="{67800E9C-1F6A-43CF-BD73-11AD9F377D14}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 7" guid="{7538C4D0-AD8C-438D-B279-4F9B4668ED47}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 4" guid="{4DADA64F-E99D-4560-8154-F4711FEFCC09}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 5" guid="{54CD2F5B-55D9-4191-B81C-1C02D9A49EAE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{6792CC1B-4085-4BCC-B147-CBA2121D3ADE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{2D114C46-41D7-4FBC-B93A-EDECFD188CDF}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{5AC41348-2849-431B-9821-2367F222BDE5}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 8" guid="{6AC71E77-F2B3-49F6-B5B5-6087FD00F176}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{5AC41348-2849-431B-9821-2367F222BDE5}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{2D114C46-41D7-4FBC-B93A-EDECFD188CDF}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{6792CC1B-4085-4BCC-B147-CBA2121D3ADE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 5" guid="{54CD2F5B-55D9-4191-B81C-1C02D9A49EAE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{4DADA64F-E99D-4560-8154-F4711FEFCC09}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 7" guid="{7538C4D0-AD8C-438D-B279-4F9B4668ED47}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 6" guid="{67800E9C-1F6A-43CF-BD73-11AD9F377D14}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3760,9 +3759,6 @@
     <t>https://media.licdn.com/dms/image/C5603AQHAKVHMG-XlCQ/profile-displayphoto-shrink_800_800/0/1624062292212?e=2147483647&amp;v=beta&amp;t=TJRWG9LrtJFEHFUiHlPI4HQ_rs-R4eQloh1vCoUPn_k</t>
   </si>
   <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBYVFRgWFhUYGBgYGhocHBoaGBoaGhoaGhgZGhgaGhgcIS4lHB4rIRgYJjgmKy8xNTU1GiQ7QDs0Py40NTEBDAwMEA8QHhISHDQkISs0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDE0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NP/AABEIAOEA4QMBIgACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAADAAECBAUGB//EAD4QAAIBAgQDBQYFAgQGAwAAAAECAAMRBBIhMQVBUSJhcYGRBhMyobHBQlLR4fByghUjM2IUkqLC0vFDU3P/xAAZAQADAQEBAAAAAAAAAAAAAAAAAQIDBAX/xAAkEQEBAAIBBAEFAQEAAAAAAAAAAQIRAxIhMUFRBBMiMmFxUv/aAAwDAQACEQMRAD8A7vcCSZARBU2sN4z1JcIJ4yCOwvDU9IaLZlOkFUblJPzMrsbxHCMg0aISTRMkgiC6xyQJUFTtCqYKmpbwl6lSAEMspieOFyVgpvJNLRSCrJ0mf3b8NZwf0ECNlgmQg/pGXEZT2tfrKx5JfKMuHKeBzTj+6Ekjgi4hdOk0Yqr04+XSGdDBssAiwFpXdekM0g0ACBrrDZ7yLCRRY5DqUg6wqiOhBholV6dpKmhtDVIki0ew8kaG0ijJL3ukdLmQppaGR7SYdSQSRQ8oNmkkeVSSsekEyQ2a8E7mRTgDU4xWJqmsiWgpFmkqVMsbep7o3lLmGTSTldTasJ1XSwiACw2EOgHlAAyylOYb26tSQ+WCqgjlLbJBuNIWDGqL09ZnYqnNhpWrJeTVbZWHrFD3dJsLWGUFdQZk11tCYB+1kvo31m3Hn6rn5cPcXXZiY6rCtTtGm7mBZYNxDMIN10gFZjaOhiZdY6qYwIBIHSPIMIgHUfeJTaM1K41vGpi0AL7zuij2EUAfPEINbwqRKTURKNY6rFlhakVKRg6qgHeTW5iamOcFKxUR1XSGAERIi0W1dkPKadNLCVwNNpaosCJnyNeLySJLlEecqobSfvLc5jHRd1bq6Ss7yD1b9fE5jK5fvvHaeMEcwDv0jtc2gHo3084tq0z676mCSpYg9CD85YxKWGnmf0EqFdD05mLG9yznZ0TMJAwVJrqveBCAmdrgMWtB1XiqGAvrHokC8MrwLr0jjSEgGKyGW0j72MKl4UIVGgUMO8CF1iCeeKTyRQCKNJ54ImQLRK0upVEODKFNrywpsIFVjOB1gKjk84switeBkidZMEDlHzCMTGkRXuINHKm0V5CoNZlzT8dtuG/lpcD6Qgbn85TRjbaG94Bqdun7czMNbdXaRaUE8/mf0gq1uglR69tQrMPIfeUH4mQdQbeH7x2dixy7+GleEaoAo8JkHHqw03kMRinAJyG0lpdJ4lySdvM7SjUzHnYHbqf27pl4/F1XBCdknW/O3dfQHY6weD4fnp2f484Of8S2A3NzqSL275cnbbDK23VjruCsWpnMSSGI1l+wmZwaoUJRjfMN+8fwzUM3wy3i5s5rIB0MCyWlpmlaoZogMiQqSTGQYSiBAMLbeO0jTuTJpj0KfWJ6NtZYQARnMC2r5j3Ro+SKAAtEEiWSCzPbVJVEkWkbxZo9p0lnEYPI5YxAgFhKmkINZVUiWKbkdIwnawlXCY5KhNmBK+I8tRDmpeVKvYRyttr+cz5d6b8Extsvn01ESV8VhmOxA7+nlB0apyI5/Eik26kAmXle475z79NtVzfEeDVqy3Ziq6hUG4BtZiDoW8esgnBkVVCnK1zop0sToD1tOqYm228jkF9BtK6u2hMe+6zOF8HCMXLE7bjY21tL3FqAKXGkuUzYQRF8w5Wgc8ubw9r6285d9wLDT0lPEoUaw5mMOJZeywAPdsZLTpTd8jXHIg+k3Wa85qvVvredDhnuinqo+k24b5jl+ox1qmaV2hKjSGXSdDlQIg3EIIzCGwF7yTpNrIOsnSSILSmKp4wDac5B303gQucRSp5xQPRLCR6VMX3lkIoN+ciRdoCU7iMUtLWeDqGOwpQb9ZCrpEFN7x2PfCUaDVxCiCOkQeMDqIzMOl4O8dVvFrfY5dXcW2pgIoG3Lu7r9IsK9t5FHYAqBe4tGdCjFW30221sdJy8mFx7uzDOZf6vtXsJTxHEVQEkyhjMblExqIaswd9E7+fhJl21skjpKXEQEzuGy2vsfK0hg+PUn2LLuLMCL+u8k2JRQASALcyBMvFVaT6A5jyCgn6CWne4bH4wPou45yg5BFib+MsiiWAyIbbXbQaXvcb8plVkLOVDhkAGq8yRrqDtF0l1buh6aMrWvdbc+XdOqwP+mn9InMIuUWnQYbFq1NcmoAA8LC2s04Zu2sPqLqSVYZpG8ysVj81Raat2t2tyUan9JopUuNZ1dNcnVEmaMDBs4OxivFobSZo6GDiYxGnUqASB1HSMoG53js14ArRSOWPADClHtrC0zeEuAdorD2BeQL63liqtxppKxWKnAqrkwRvLDxZJOj2rqDCInfLmHwbvsLDqYXFYEojPfNlBNgLXtLkqbYo5IegjN8Kk26Q+DNNlDAFgRvf7SK8TVHNOxBb4SfS0qY0rkt4DD63bS2tuv7SPG02brp9x94XAowzs27MQO5F0X11b+6Q43f3LMPw2byU9r/pvFnjvGxXHl05SsFgpNmlZ+FI4yhmAFtASNO6TxFxz0OxksKx5zz/D0d7PguB0UfOAQbjnmBt3N5zVdwgGTJoSfgta978+pkUS4g6mHzTTHOlcJbus3Evm+NmYHXKLKvyFyPEmUlpgbC01Xw/fKdRAp+cMstq6dTt2Co08zqO/5CQqH3eJNhZX1tyubk26a30lzAfiPkPv9pHiigqWI1QE3G4t2vtOvhw6cdvO58urLTmOE4nLVeo55lb95P7Tr0qX1v3zgEqf5DdTV+wM6dMR/kA9wE1jCtGlUBzG8bhWIzIWvftNY9Re15g4yo9lpI2UkWPnvNaifdoqrsBYCMNNqwH7R80p5zvz2A+pk6L3uD5d8nLHts8aIx6QiSKLHY2kLTvFK+fvigS5SqSyovzmb7zoDD4dzfWJWll0MER0k6la+kGzR0Qy77XM08Pw+wzOLnkvLz6yHD6aKbsRnOwPL95ps145j8lb8K1Kpe/0HKPVbskE3B01+kDiQV7Q3H8sZUrVPeLddxsO8b+XKXpDAw+KOGrmm/wMbrz3mjxunnCVE3R1N+eXML/b0lbjeDFajmX407Q66fEsj7NY/wB4pR9xHoOvYxnAKkHY6HzkC0cNJDkcE+r0m+Km2Q35ruh77qR5gyVdGTVNRzB+0qe1hOGxCYkfA4CVB4G6nyv85eSsrAFTcHW/KcPJj05WenoceXVjPlHDcZXZ+ye/9Zc/xEDW4I7pRxGHpasyjSYRpi5bMACdFB2EnU9LmVjfrcTQ7ETD4xxpUXMRe5sAOZ+wgWYE6aCcz7R4rM6oORH1lTGbLPO6d/wquWpox3IufEyzXGZSOoI9Zm8ENqKeH3mipno4+I83LzXn9dWSmysLEV2Hy08tJu8JxQdFQ/hN/IRvavDgBXA3cZvHKQD6WHlM3h+YFwupyPbxym0nxR6aXC7uWqnmSF+/2E2cIme7nYaDwG59fpMqg2RAi/hGUd5/9zbwCbLyW1+9v5rGS5RoX1PP5DpFXp5dRL9NNIOvTuLRhUD6SFRtJBDy6SLmY2a7NJ3K0UhmiiNpJR5xnNoR300gZetFsRXHSEw6ZmUd/wBIBNJYwDdsef0iobi0gRa0DVVl6kd24/WFSsv5h5m0KWB2MpLOqMDqdQefI+PQyq9l+HQj0Il2utrkDfccj+/fMytUF7Dyvv5fpKhUKo4Q+8A7P/yL0G2ceHPqPCYlJfc4opt2hbvVz2T9psmpzGpHLkRzEpYzBF62EqILgNkf+lQXUnwKAf3SqTqRHvGEgzSTZvtBgVr0XQ8wbdx5GefezvFGpOaNT8Jt4ETqPav2uTCjIgD1Dpl/Cne5+2/hON9/h8Qor1HWnW/EEJBa2xyMuXbo3KY8uMy/1rxZ9Lr+KsCnZ1vzmAUygEg3+kLh8YURbsHRh2W+xF9DBVsQLabzm6bj2rq6plNw1WrlQmY/CuDGuzV6hCUluQzGwNudz+EdZotRDkK1yoF3sbdn8oPInb1g8XmxL06Z0QuFVF0VVUHYfea8ePbqrDly9RfT2lpIAMrBLkBx47ldxNzC4lXUMrBlOxBuD5zg8fw5gjqNlcr6bfSZuEx1bDsMjEC9ip1UkatcdxNpvM7PLCyV6djcMKiMjbMPQ7g+RnOYTDMlSzfhBv5C/wBoqHtYVCe8oHtnKCjaX8GH3m0tUVdfdOtvxHLYjnsbn0l9qnwyaDFivr4nl851vDaFgB6n6mcz7OqGCkn4Lg/2kidRnDstNTZbZmI3I5DuvGGgMQmwa9ugJt6RmqqTYHX6eMKGVF0AAHKVVOpc7zLk5JjP614+O5X+A1igLD8XTxmdVgMRjCahIUsDpcd231lp02J562im8pKLJjbIBkMULrFDRbXmaINBZoUNNNJImWMC1nX09ZWEiHsQekjLsqOop2O4EIUA2A8pXwxzAHYEXh2aUmK1cjnpMPiFO+oJNtel7fzfcTYxIfcajpz/AHlFgDodDKiaxlxQOoP63G4I+U0OC1wXcbhLMO4tcfSZONoizOgs4+JetufebDzmfgMXUQlEa3vc5JA7Qyp2bHoPvKDtMfxOlRW9R1ToCdT4DcziPan2prMoXDjIjbufjPcBsv18JzPtHhHDe8JZj+IsST3G5nQ8O4YMRgg6Ht2JHcyk6fK0i+4HLYeoHXI6Ehrg9b9decjU4a1ygWzIB3ZgdmAnX+yq06iOrp201IIBOnxG03uN8OpvSTE0rZqQs69UOjDy0PnM5O/dW3m3CnZTlNyp3X7joZp4ij7p+3cC11v0+xlzFYdEdHGzG3hfYzTx2CWuv+YSVAtYac9CDvfl5mPPi6orDk6azMOxKBjpn7X9uy/S/nM7grk1y4+GiC3mdvWxmpxVsiE7bAAchyHhy8ovZikowmIe12aoo8lXN9Y7OmSFb1W1LiCCm7M4uEUvb8zuRkXxNwPWZlTgzEoNyq9o9WOrHzJM0eKg1cZRpHYOGf8AqUXsf6QCPEmdJVppTDFjvc/tKxx2i1x3HcNkTCrbepf5gfedotMKnlOT9p3zV8KlrHsG39TradbjmypKnmi+HGcAr5DiUP4SCPNnB+gnVcIft1G7wg8FE43DVCmKdABaoU1PQMC1u+2b0nZcOplVJO7Et4XN7TLk5OnH+tePDqy/jXZ7ypjC7KVUhb9ZJmNv5eDLWtp8pwXK27ruxxkmojhMGiAX7R6nr4RYt+ajxklDbt8zeTQr4x9eW97HRjrWmZ79opr5V6R5X3MvkvtY/CqI95NAIjO7bgBZjFS3F9ri/hzjtIGTabq6YNrjbpDIT4fSQwhui/0j6QzSkAu5Ez+J4pFQkrryt1l6s8y8Vhg24jgc/iKpch0IV1GxNg4/KT9+U51MZfEplFgEdrdM2UAfWdJj8CF11E5OpTyYlm5Oot9/nKpNzForqcwvcWkPYTEW95S5Brj6H7QYe6zN4HiPd1if931MdDpcZRbD1xXRbg/Gv5utu/6zdwzUWHvaLj3dRSlSmx+En4bg6ixJH/qVMQ4dbHnzlLD4Js2akLtazC3YcdG5ScsdiVzHGrpTZDulS3fz/SbeDq56Sevpp+s6KnwqnUV1r4cWa1znu2YC1wRty/eSw/BqFNMiI+lxdnvodeVusUyo05k8LbEuKSEDUEk7Afr3S3xPCjBKqJ2lGZs2ljUbIAT3AKLDqJ02FwqIDlTtHyE5vimFes7K5NkaxtsdNAO6xkZ5a73wvHG5doocBwYQtiamgCkJfck7mFwtUVqud/gXUC2/QS7TwSAAEXA2B1t3W2lgIBsLfzpMr9T/AMxtPp/msLGcJeriRiLgBGUqvXIbgHpNerhXqau+n5V0HruZbRPKSK21HnMbzZX21x4cZ6UqPDkQ3Ci/Urc/PWXUtBs8G1hrM97vdrrU7LhYQVQC172kUfTpE6A6nWGhLVdai3OtxyhlYHbWVq+HueVj1k0QLtp1Ai0cqzlPT+ekUB/y+sUNK3UwpkxTk1Maei8wJkkiukTvICoJJumwh7CgflH0hnNhbrA4NuwvgPpLNry0Ae7mTxLiqJ2Qpdug69JsYusqKSTaY6YdiLge7XrYe8b/AMR8/CVCrGfFYmoQpw6gNsGcAnyIvMTG8AdHZg673yM3wnmFbpOyxIFFOyO2/PdgPE6kyvgeClmD1etwn3b9IwxcN7PVygY5AD1bW3XQQ3D/AGOTMXqOxJOy9kepuT8p2ZXSQC6xbCtRwaIOyg066n5w5Pr9ITLKzPZoAULpEUuDbcayR2j4bUt4D7wMKi9/ETFxP+u4J0OU/wDSB9pqYh8j5h5zCrVgarnrYegmPPPxbcH7D1rAjlBE/sYKu/UwT4oW7xOLTtXgbjWBq4pU537pnPiCee8q1X5mGi2v1OJH8KwX/GMx10mJiuIomhbXoNTKP+LOSMiMfHe00x47WeXLI7PD1+sN74HnOcw7Yh2ORLIds57XnlFpHEU8ch1pDLzcEsB5KM3yml4svhH3Z8t+ue+U3c30I85HCYX3oB/4kA21GQprysWk19lWZv8AXq33ByJl9RmEJwZe03nnoP3h/Ovr+8Uvf4DW/wDsr/8ANSil/YL79aSPGLEQavYyJeasU3XMJRqGxloHpBVad5Bui4RWzU17hb00lzFYpaaZm7gAN2Y6KoHUmYvA6tsyeY+/2l80i9dSfgpi4H+9tAfIX9ZpO8RfKzSwxJDvq/Ick7l7++TdbnXaWLwFQ/z+eUAptQzVizbIB6y2I1Ua+Nr+URaUCZpBT2rd0anrcnYSqtdffAE9pgbDuGv2gS+475RrJrLzrKlRYoKYMbQa4sIDZGY66AdBfVthJLTvIOhysBfUb326EeYEoMqpxRHawZQx/Dc38NQDMU1szsR1h62IRqZdkAdGsDb8XUTOWoB6fec/1GU7Yujgx81dq1P55wFd5UrYoDUmQQO+uwPrOfHjyy8N8s8cfItTEAWF/Ian0lvCcGqYgdolE7viPnLfCuEi97anfqfGdXhqAUTpx4ccfLmy5rl4eZf4I6VTSYDMOfIjk06vh3s8qAFtTNLjmBzgOg7aa+K8x94LCO7r2ny9yKL+bPf5ATaRlav0cKq7C0l79Ngcx6KM3zGg84kwibtdz/vYt8ibfKHuBoB9hGQDYQNqVy99+1520g0wuU9O8afT7y4GPcI3jrDYDs35j6R4/ux3+pihsOaKneHRgYAGSRZntoMiC95Cs8iQbxEHpJoTwNTK4Pfr4HQzqaHM+HynJFG6ToMDiMyA89mHeI8cpe2xljZ3saJeVqb3Zv8AbYfK/wB5JanWBw/4j1YmXpmO7awTtfQbmM7QGLxQpLfdzsOkcgR4txFaKZRq/Id85/glN2rrVe5a58rgj7w64VnJdzbnc8on4mlMqqC9mFz3X1laLbqrwNRZPMCBaQd9pEMyiDrJ95Knooju0YcJ7RVgjKuwN2+dvX9ZhVsU7XCDTqf0nZe1WDDIGUXKm+m45N5fpOWRQT3Tk5prJ18PfE3DqOYXb4xowPyI7jOi4Zhc2+/0nPPUKOHXluOo6TqOD11axXY/y034cpcde2PLjZk6LC0Ao0h4KnU0hF1M0ZJKbkzmKNRcxHQkehIm7j8YtFHdjoNu8nYTiMDjAX3vm+plQq6/DVrS4r3mBTrEdfUS7TxXj6w0NtRjIPUA3IHnKZa+p+sHbuHpDQ2t/wDEr1EUB7zuHoP0ihobZayI3iimLVI7w9HceMUUm+DnmI1vjH931E0eFbN4j6RRTHh/Z08/6rskm0UU7HCinxCZHEv9bzEUUcCHGfgnO0fijxSk+3dYP4E/pH0koopCkH5+AiHwnx+0UUAyeJfC/wDS/wD3TiF5R4pzfUeY6vp/FRqc/Oa3st8HmYoouD9j5/DsMPzluntFFOtyOe9r/gT/APT/ALWmBhvjHjFFGGrU3EtUY8UolsSQiiiCMUUUA//Z</t>
-  </si>
-  <si>
     <t>https://d3wnzga3fpd9a.cloudfront.net/photos/Dr-Allison-Beardsley-DC-316262-circle_large__v2__.png</t>
   </si>
   <si>
@@ -3791,6 +3787,9 @@
   </si>
   <si>
     <t>Pain</t>
+  </si>
+  <si>
+    <t>https://d2uur722ua7fvv.cloudfront.net/0cbb183b-23cf-4ee8-8e6f-4c6f58a4d92dzoom.jpg</t>
   </si>
 </sst>
 </file>
@@ -4295,7 +4294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4698,7 +4697,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4717,7 +4715,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="References_Email QA_Status"/>
@@ -4932,8 +4930,8 @@
   </sheetPr>
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4949,7 +4947,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -5010,13 +5008,13 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A2" s="168">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="168" t="s">
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -5044,7 +5042,7 @@
         <v>22</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="M2" s="10"/>
       <c r="N2" s="9" t="s">
@@ -5066,19 +5064,19 @@
         <v>80220</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>1227</v>
+        <v>1237</v>
       </c>
       <c r="U2" s="11"/>
       <c r="V2" s="7"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A3" s="168">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="168" t="s">
+      <c r="C3" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -5136,13 +5134,13 @@
       <c r="V3" s="13"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A4" s="168">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="168" t="s">
+      <c r="C4" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -5200,13 +5198,13 @@
       <c r="V4" s="13"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A5" s="168">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="168" t="s">
+      <c r="C5" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -5258,19 +5256,19 @@
         <v>80401</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="U5" s="11"/>
       <c r="V5" s="13"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A6" s="168">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>1236</v>
-      </c>
-      <c r="C6" s="168" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -5326,13 +5324,13 @@
       <c r="V6" s="13"/>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A7" s="168">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>1236</v>
-      </c>
-      <c r="C7" s="168" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -5388,13 +5386,13 @@
       <c r="V7" s="13"/>
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A8" s="168">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="168" t="s">
+      <c r="C8" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -5450,13 +5448,13 @@
       <c r="V8" s="13"/>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A9" s="168">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="168" t="s">
+      <c r="C9" s="7" t="s">
         <v>60</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -5512,13 +5510,13 @@
       <c r="V9" s="7"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A10" s="168">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="168" t="s">
+      <c r="C10" s="7" t="s">
         <v>63</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -5572,13 +5570,13 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A11" s="168">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>1232</v>
-      </c>
-      <c r="C11" s="168" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -5634,13 +5632,13 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A12" s="168">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="168" t="s">
+      <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -5696,13 +5694,13 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A13" s="168">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="168" t="s">
+      <c r="C13" s="7" t="s">
         <v>86</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -5752,17 +5750,17 @@
         <v>80209</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A14" s="168">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="168" t="s">
+      <c r="C14" s="7" t="s">
         <v>93</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -5818,13 +5816,13 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A15" s="168">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="168" t="s">
+      <c r="C15" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -5873,17 +5871,17 @@
         <v>80033</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A16" s="168">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C16" s="168" t="s">
+      <c r="C16" s="7" t="s">
         <v>108</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -5939,13 +5937,13 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A17" s="168">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="168" t="s">
+      <c r="C17" s="7" t="s">
         <v>115</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -6001,13 +5999,13 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A18" s="168">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C18" s="168" t="s">
+      <c r="C18" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -6035,16 +6033,16 @@
         <v>22</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="Q18" s="7" t="s">
         <v>25</v>
@@ -6061,13 +6059,13 @@
       <c r="U18" s="13"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A19" s="168">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C19" s="168" t="s">
+      <c r="C19" s="7" t="s">
         <v>126</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -6095,7 +6093,7 @@
         <v>22</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="N19" s="12" t="s">
         <v>129</v>
@@ -6121,13 +6119,13 @@
       <c r="U19" s="13"/>
     </row>
     <row r="20" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A20" s="168">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="168" t="s">
+      <c r="C20" s="7" t="s">
         <v>133</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -6181,13 +6179,13 @@
       <c r="U20" s="13"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A21" s="168">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="168" t="s">
+      <c r="C21" s="7" t="s">
         <v>140</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -6241,13 +6239,13 @@
       <c r="U21" s="13"/>
     </row>
     <row r="22" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A22" s="168">
+      <c r="A22" s="7">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C22" s="168" t="s">
+      <c r="C22" s="7" t="s">
         <v>142</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -6301,13 +6299,13 @@
       <c r="U22" s="13"/>
     </row>
     <row r="23" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A23" s="168">
+      <c r="A23" s="7">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C23" s="168" t="s">
+      <c r="C23" s="7" t="s">
         <v>148</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -26645,37 +26643,37 @@
   </sheetData>
   <autoFilter ref="A7:AE160" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <customSheetViews>
-    <customSheetView guid="{2D114C46-41D7-4FBC-B93A-EDECFD188CDF}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{67800E9C-1F6A-43CF-BD73-11AD9F377D14}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A7:AE160" xr:uid="{BDB767A1-604B-4A4C-A462-99084C4EBA19}"/>
+      <autoFilter ref="A7:AE160" xr:uid="{988362AA-6051-794A-8C95-70A73A65EEDD}"/>
+    </customSheetView>
+    <customSheetView guid="{54CD2F5B-55D9-4191-B81C-1C02D9A49EAE}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AE160" xr:uid="{E7704B95-8026-514E-81A8-B199FFAF6A2F}"/>
+    </customSheetView>
+    <customSheetView guid="{4DADA64F-E99D-4560-8154-F4711FEFCC09}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AE160" xr:uid="{C9068A5D-0C71-074B-BBD1-2A6632D8113E}"/>
+    </customSheetView>
+    <customSheetView guid="{7538C4D0-AD8C-438D-B279-4F9B4668ED47}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A7:AE160" xr:uid="{C6611655-5BB5-F54B-9210-DFB5B6E8592D}"/>
+    </customSheetView>
+    <customSheetView guid="{6AC71E77-F2B3-49F6-B5B5-6087FD00F176}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A7:AE160" xr:uid="{299804DB-1348-ED45-9866-DA574896B68E}"/>
+    </customSheetView>
+    <customSheetView guid="{6792CC1B-4085-4BCC-B147-CBA2121D3ADE}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A7:AE160" xr:uid="{919453F7-C978-A048-A586-BA6E1B74A7AC}"/>
     </customSheetView>
     <customSheetView guid="{5AC41348-2849-431B-9821-2367F222BDE5}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AE160" xr:uid="{70FB37EC-2860-114C-9EB3-351CBF0C7981}"/>
+      <autoFilter ref="A1:AE160" xr:uid="{AD7B327C-2A8B-1247-ABD6-E7ED24C75750}"/>
     </customSheetView>
-    <customSheetView guid="{6792CC1B-4085-4BCC-B147-CBA2121D3ADE}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{2D114C46-41D7-4FBC-B93A-EDECFD188CDF}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A7:AE160" xr:uid="{3BA0482C-BA2E-C94E-BD84-11A4ECB93D34}"/>
-    </customSheetView>
-    <customSheetView guid="{6AC71E77-F2B3-49F6-B5B5-6087FD00F176}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A7:AE160" xr:uid="{66762E82-92AE-2943-9B7F-8A88CED99A40}"/>
-    </customSheetView>
-    <customSheetView guid="{7538C4D0-AD8C-438D-B279-4F9B4668ED47}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A7:AE160" xr:uid="{ECA257E8-5287-E947-AEEF-9A72092C8C9E}"/>
-    </customSheetView>
-    <customSheetView guid="{4DADA64F-E99D-4560-8154-F4711FEFCC09}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AE160" xr:uid="{2306CAE8-DA62-504D-82A7-AE4B0D8129C3}"/>
-    </customSheetView>
-    <customSheetView guid="{54CD2F5B-55D9-4191-B81C-1C02D9A49EAE}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AE160" xr:uid="{A4B45B47-9F70-044B-A065-03313D831D00}"/>
-    </customSheetView>
-    <customSheetView guid="{67800E9C-1F6A-43CF-BD73-11AD9F377D14}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A7:AE160" xr:uid="{C6730C3F-C52D-CC4D-9B49-2ED69FE69236}"/>
+      <autoFilter ref="A7:AE160" xr:uid="{DAE2D3E1-0472-6E48-84D1-237F875CC488}"/>
     </customSheetView>
   </customSheetViews>
   <dataValidations count="3">

</xml_diff>

<commit_message>
updated db to include new headshot of practitioner mike viscarelli
</commit_message>
<xml_diff>
--- a/public/data/practitioners.xlsx
+++ b/public/data/practitioners.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianlalli/Desktop/Natu.Health/Natu.Health/public/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianlalli/Desktop/Moon Rooster Projects/Natu.Health/Natu.Health/public/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F5A9CB-9E38-9042-BC3F-AD1770D76099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAEFBAF-4B3B-3744-999D-A95C1F72F28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="1640" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,14 +38,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 8" guid="{6AC71E77-F2B3-49F6-B5B5-6087FD00F176}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{5AC41348-2849-431B-9821-2367F222BDE5}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{2D114C46-41D7-4FBC-B93A-EDECFD188CDF}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{6792CC1B-4085-4BCC-B147-CBA2121D3ADE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 5" guid="{54CD2F5B-55D9-4191-B81C-1C02D9A49EAE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 4" guid="{4DADA64F-E99D-4560-8154-F4711FEFCC09}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 7" guid="{7538C4D0-AD8C-438D-B279-4F9B4668ED47}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 6" guid="{67800E9C-1F6A-43CF-BD73-11AD9F377D14}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 7" guid="{7538C4D0-AD8C-438D-B279-4F9B4668ED47}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{4DADA64F-E99D-4560-8154-F4711FEFCC09}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 5" guid="{54CD2F5B-55D9-4191-B81C-1C02D9A49EAE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{6792CC1B-4085-4BCC-B147-CBA2121D3ADE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{2D114C46-41D7-4FBC-B93A-EDECFD188CDF}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{5AC41348-2849-431B-9821-2367F222BDE5}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 8" guid="{6AC71E77-F2B3-49F6-B5B5-6087FD00F176}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3012" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3012" uniqueCount="1237">
   <si>
     <t>Clinic/s</t>
   </si>
@@ -3706,9 +3706,6 @@
   </si>
   <si>
     <t>https://d2uur722ua7fvv.cloudfront.net/photos/Dr-Weston-Nemitz-DC-316260-circle_large__v3__.png</t>
-  </si>
-  <si>
-    <t>https://scontent.fabe1-1.fna.fbcdn.net/v/t1.6435-1/161813394_126056496192817_3762082598690142724_n.jpg?stp=c0.0.120.120a_cp0_dst-jpg_e15_p120x120_q65&amp;_nc_cat=109&amp;ccb=1-7&amp;_nc_sid=db1b99&amp;_nc_ohc=O7MxukNWdlMAX-ahpLd&amp;_nc_ht=scontent.fabe1-1.fna&amp;oh=00_AfBWhQyzWU_7-w325ScHDQuVmt9xu_iwp7GvIvVguSnfVQ&amp;oe=6586D933</t>
   </si>
   <si>
     <t>https://cdn.shortpixel.ai/spai/w_447+q_lossy+ret_img+to_webp/elevationcw.com/wp-content/uploads/2020/06/Dr-Jeffrey.jpg</t>
@@ -4930,8 +4927,8 @@
   </sheetPr>
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4947,7 +4944,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -5042,7 +5039,7 @@
         <v>22</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="M2" s="10"/>
       <c r="N2" s="9" t="s">
@@ -5064,7 +5061,7 @@
         <v>80220</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="U2" s="11"/>
       <c r="V2" s="7"/>
@@ -5192,7 +5189,7 @@
         <v>80401</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>1210</v>
+        <v>1236</v>
       </c>
       <c r="U4" s="11"/>
       <c r="V4" s="13"/>
@@ -5256,7 +5253,7 @@
         <v>80401</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="U5" s="11"/>
       <c r="V5" s="13"/>
@@ -5266,7 +5263,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>42</v>
@@ -5318,7 +5315,7 @@
         <v>80246</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="U6" s="11"/>
       <c r="V6" s="13"/>
@@ -5328,7 +5325,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>49</v>
@@ -5380,7 +5377,7 @@
         <v>80246</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="U7" s="11"/>
       <c r="V7" s="13"/>
@@ -5442,7 +5439,7 @@
         <v>80111</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="U8" s="11"/>
       <c r="V8" s="13"/>
@@ -5504,7 +5501,7 @@
         <v>80111</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="U9" s="11"/>
       <c r="V9" s="7"/>
@@ -5566,7 +5563,7 @@
         <v>80246</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1">
@@ -5574,7 +5571,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>70</v>
@@ -5628,7 +5625,7 @@
         <v>80214</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1">
@@ -5690,7 +5687,7 @@
         <v>80003</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1">
@@ -5750,7 +5747,7 @@
         <v>80209</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1">
@@ -5812,7 +5809,7 @@
         <v>80215</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1">
@@ -5871,7 +5868,7 @@
         <v>80033</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1">
@@ -5933,7 +5930,7 @@
         <v>80033</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" customHeight="1">
@@ -5995,7 +5992,7 @@
         <v>80214</v>
       </c>
       <c r="T17" s="7" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" customHeight="1">
@@ -6033,16 +6030,16 @@
         <v>22</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="Q18" s="7" t="s">
         <v>25</v>
@@ -6054,7 +6051,7 @@
         <v>80211</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U18" s="13"/>
     </row>
@@ -6093,7 +6090,7 @@
         <v>22</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="N19" s="12" t="s">
         <v>129</v>
@@ -6114,7 +6111,7 @@
         <v>80004</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="U19" s="13"/>
     </row>
@@ -6174,7 +6171,7 @@
         <v>80138</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="U20" s="13"/>
     </row>
@@ -6234,7 +6231,7 @@
         <v>80138</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="U21" s="13"/>
     </row>
@@ -6294,7 +6291,7 @@
         <v>80203</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="U22" s="13"/>
     </row>
@@ -6354,7 +6351,7 @@
         <v>80203</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="U23" s="13"/>
     </row>
@@ -26643,37 +26640,37 @@
   </sheetData>
   <autoFilter ref="A7:AE160" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <customSheetViews>
-    <customSheetView guid="{67800E9C-1F6A-43CF-BD73-11AD9F377D14}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{2D114C46-41D7-4FBC-B93A-EDECFD188CDF}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A7:AE160" xr:uid="{988362AA-6051-794A-8C95-70A73A65EEDD}"/>
+      <autoFilter ref="A7:AE160" xr:uid="{B2988157-0845-6949-82F0-2A6E0ACA42AB}"/>
+    </customSheetView>
+    <customSheetView guid="{5AC41348-2849-431B-9821-2367F222BDE5}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AE160" xr:uid="{95E8F01B-00F6-4E4A-A903-345FF16E17B5}"/>
+    </customSheetView>
+    <customSheetView guid="{6792CC1B-4085-4BCC-B147-CBA2121D3ADE}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A7:AE160" xr:uid="{7670EC17-CE24-AB40-AA79-AE21129C3231}"/>
+    </customSheetView>
+    <customSheetView guid="{6AC71E77-F2B3-49F6-B5B5-6087FD00F176}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A7:AE160" xr:uid="{4934486A-C687-0C40-86D0-DFF245102870}"/>
+    </customSheetView>
+    <customSheetView guid="{7538C4D0-AD8C-438D-B279-4F9B4668ED47}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A7:AE160" xr:uid="{ABF9EDED-836B-C74B-9DEF-AE70BAAB393B}"/>
+    </customSheetView>
+    <customSheetView guid="{4DADA64F-E99D-4560-8154-F4711FEFCC09}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AE160" xr:uid="{297320EF-E1F4-F249-854F-927A80BB2499}"/>
     </customSheetView>
     <customSheetView guid="{54CD2F5B-55D9-4191-B81C-1C02D9A49EAE}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AE160" xr:uid="{E7704B95-8026-514E-81A8-B199FFAF6A2F}"/>
+      <autoFilter ref="A1:AE160" xr:uid="{B3A7754F-FBD0-4B41-A076-E7D9C5927B9C}"/>
     </customSheetView>
-    <customSheetView guid="{4DADA64F-E99D-4560-8154-F4711FEFCC09}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{67800E9C-1F6A-43CF-BD73-11AD9F377D14}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AE160" xr:uid="{C9068A5D-0C71-074B-BBD1-2A6632D8113E}"/>
-    </customSheetView>
-    <customSheetView guid="{7538C4D0-AD8C-438D-B279-4F9B4668ED47}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A7:AE160" xr:uid="{C6611655-5BB5-F54B-9210-DFB5B6E8592D}"/>
-    </customSheetView>
-    <customSheetView guid="{6AC71E77-F2B3-49F6-B5B5-6087FD00F176}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A7:AE160" xr:uid="{299804DB-1348-ED45-9866-DA574896B68E}"/>
-    </customSheetView>
-    <customSheetView guid="{6792CC1B-4085-4BCC-B147-CBA2121D3ADE}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A7:AE160" xr:uid="{919453F7-C978-A048-A586-BA6E1B74A7AC}"/>
-    </customSheetView>
-    <customSheetView guid="{5AC41348-2849-431B-9821-2367F222BDE5}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AE160" xr:uid="{AD7B327C-2A8B-1247-ABD6-E7ED24C75750}"/>
-    </customSheetView>
-    <customSheetView guid="{2D114C46-41D7-4FBC-B93A-EDECFD188CDF}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A7:AE160" xr:uid="{DAE2D3E1-0472-6E48-84D1-237F875CC488}"/>
+      <autoFilter ref="A7:AE160" xr:uid="{5ABF1267-CA14-6245-B311-CD5D4B8703F1}"/>
     </customSheetView>
   </customSheetViews>
   <dataValidations count="3">

</xml_diff>